<commit_message>
lOAD AND PROCESS data
</commit_message>
<xml_diff>
--- a/data/Course_output_data.xlsx
+++ b/data/Course_output_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OVGU\DE\4th_sem\Software_Project_AI_Lab\AI_Thematic_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144FF6EA-FD0F-4C52-AC3B-78E5533AC85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F00720D-0B64-46F8-9F6B-9A4F58A6E091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="1105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="1107">
   <si>
     <t>Serial number</t>
   </si>
@@ -3337,7 +3337,13 @@
     <t>Social Sciences &amp; Humanities; Natural Sciences</t>
   </si>
   <si>
-    <t>Computer Science &amp; Data; Statistics &amp; Data Analysis</t>
+    <t>keywords_processed</t>
+  </si>
+  <si>
+    <t>embeddings_processed</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -3722,10 +3728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="M74" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S89" sqref="S2:T89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3735,12 +3741,12 @@
     <col min="6" max="6" width="20.88671875" customWidth="1"/>
     <col min="7" max="7" width="56" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.88671875" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" customWidth="1"/>
+    <col min="9" max="10" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" customWidth="1"/>
     <col min="12" max="12" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3795,8 +3801,14 @@
       <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>1105</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3852,8 +3864,14 @@
       <c r="R2" t="s">
         <v>297</v>
       </c>
+      <c r="S2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3909,8 +3927,14 @@
       <c r="R3" t="s">
         <v>304</v>
       </c>
+      <c r="S3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3966,8 +3990,14 @@
       <c r="R4" t="s">
         <v>312</v>
       </c>
+      <c r="S4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4023,8 +4053,14 @@
       <c r="R5" t="s">
         <v>319</v>
       </c>
+      <c r="S5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4080,8 +4116,14 @@
       <c r="R6" t="s">
         <v>326</v>
       </c>
+      <c r="S6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4137,8 +4179,14 @@
       <c r="R7" t="s">
         <v>333</v>
       </c>
+      <c r="S7" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4194,8 +4242,14 @@
       <c r="R8" t="s">
         <v>341</v>
       </c>
+      <c r="S8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4251,8 +4305,14 @@
       <c r="R9" t="s">
         <v>348</v>
       </c>
+      <c r="S9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4308,8 +4368,14 @@
       <c r="R10" t="s">
         <v>41</v>
       </c>
+      <c r="S10" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4365,8 +4431,14 @@
       <c r="R11" t="s">
         <v>355</v>
       </c>
+      <c r="S11" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4422,8 +4494,14 @@
       <c r="R12" t="s">
         <v>362</v>
       </c>
+      <c r="S12" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4479,8 +4557,14 @@
       <c r="R13" t="s">
         <v>369</v>
       </c>
+      <c r="S13" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4536,8 +4620,14 @@
       <c r="R14" t="s">
         <v>56</v>
       </c>
+      <c r="S14" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4593,8 +4683,14 @@
       <c r="R15" t="s">
         <v>376</v>
       </c>
+      <c r="S15" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4650,8 +4746,14 @@
       <c r="R16" t="s">
         <v>384</v>
       </c>
+      <c r="S16" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T16" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4707,8 +4809,14 @@
       <c r="R17" t="s">
         <v>391</v>
       </c>
+      <c r="S17" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4764,8 +4872,14 @@
       <c r="R18" t="s">
         <v>398</v>
       </c>
+      <c r="S18" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T18" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4821,8 +4935,14 @@
       <c r="R19" t="s">
         <v>405</v>
       </c>
+      <c r="S19" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T19" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4878,8 +4998,14 @@
       <c r="R20" t="s">
         <v>412</v>
       </c>
+      <c r="S20" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T20" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4935,8 +5061,14 @@
       <c r="R21" t="s">
         <v>420</v>
       </c>
+      <c r="S21" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T21" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4992,8 +5124,14 @@
       <c r="R22" t="s">
         <v>427</v>
       </c>
+      <c r="S22" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T22" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5049,8 +5187,14 @@
       <c r="R23" t="s">
         <v>434</v>
       </c>
+      <c r="S23" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T23" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5106,8 +5250,14 @@
       <c r="R24" t="s">
         <v>441</v>
       </c>
+      <c r="S24" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T24" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5163,8 +5313,14 @@
       <c r="R25" t="s">
         <v>85</v>
       </c>
+      <c r="S25" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T25" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5220,8 +5376,14 @@
       <c r="R26" t="s">
         <v>448</v>
       </c>
+      <c r="S26" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T26" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5277,8 +5439,14 @@
       <c r="R27" t="s">
         <v>454</v>
       </c>
+      <c r="S27" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T27" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5334,8 +5502,14 @@
       <c r="R28" t="s">
         <v>461</v>
       </c>
+      <c r="S28" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T28" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5391,8 +5565,14 @@
       <c r="R29" t="s">
         <v>468</v>
       </c>
+      <c r="S29" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T29" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5448,8 +5628,14 @@
       <c r="R30" t="s">
         <v>475</v>
       </c>
+      <c r="S30" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T30" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5505,8 +5691,14 @@
       <c r="R31" t="s">
         <v>483</v>
       </c>
+      <c r="S31" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T31" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5562,8 +5754,14 @@
       <c r="R32" t="s">
         <v>491</v>
       </c>
+      <c r="S32" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T32" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5619,8 +5817,14 @@
       <c r="R33" t="s">
         <v>498</v>
       </c>
+      <c r="S33" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T33" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5676,8 +5880,14 @@
       <c r="R34" t="s">
         <v>506</v>
       </c>
+      <c r="S34" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T34" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5733,8 +5943,14 @@
       <c r="R35" t="s">
         <v>514</v>
       </c>
+      <c r="S35" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T35" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5790,8 +6006,14 @@
       <c r="R36" t="s">
         <v>523</v>
       </c>
+      <c r="S36" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T36" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5847,8 +6069,14 @@
       <c r="R37" t="s">
         <v>531</v>
       </c>
+      <c r="S37" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T37" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5904,8 +6132,14 @@
       <c r="R38" t="s">
         <v>539</v>
       </c>
+      <c r="S38" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T38" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5961,8 +6195,14 @@
       <c r="R39" t="s">
         <v>549</v>
       </c>
+      <c r="S39" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T39" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6018,8 +6258,14 @@
       <c r="R40" t="s">
         <v>558</v>
       </c>
+      <c r="S40" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T40" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6075,8 +6321,14 @@
       <c r="R41" t="s">
         <v>566</v>
       </c>
+      <c r="S41" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T41" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6132,8 +6384,14 @@
       <c r="R42" t="s">
         <v>575</v>
       </c>
+      <c r="S42" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T42" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6189,8 +6447,14 @@
       <c r="R43" t="s">
         <v>584</v>
       </c>
+      <c r="S43" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T43" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6246,8 +6510,14 @@
       <c r="R44" t="s">
         <v>593</v>
       </c>
+      <c r="S44" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T44" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6303,8 +6573,14 @@
       <c r="R45" t="s">
         <v>602</v>
       </c>
+      <c r="S45" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T45" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6360,8 +6636,14 @@
       <c r="R46" t="s">
         <v>611</v>
       </c>
+      <c r="S46" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T46" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6417,8 +6699,14 @@
       <c r="R47" t="s">
         <v>620</v>
       </c>
+      <c r="S47" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T47" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6474,8 +6762,14 @@
       <c r="R48" t="s">
         <v>628</v>
       </c>
+      <c r="S48" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T48" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6531,8 +6825,14 @@
       <c r="R49" t="s">
         <v>636</v>
       </c>
+      <c r="S49" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T49" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6588,8 +6888,14 @@
       <c r="R50" t="s">
         <v>644</v>
       </c>
+      <c r="S50" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T50" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6645,8 +6951,14 @@
       <c r="R51" t="s">
         <v>652</v>
       </c>
+      <c r="S51" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T51" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6702,8 +7014,14 @@
       <c r="R52" t="s">
         <v>661</v>
       </c>
+      <c r="S52" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T52" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6759,8 +7077,14 @@
       <c r="R53" t="s">
         <v>669</v>
       </c>
+      <c r="S53" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T53" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6816,8 +7140,14 @@
       <c r="R54" t="s">
         <v>678</v>
       </c>
+      <c r="S54" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T54" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6873,8 +7203,14 @@
       <c r="R55" t="s">
         <v>687</v>
       </c>
+      <c r="S55" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T55" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6930,8 +7266,14 @@
       <c r="R56" t="s">
         <v>695</v>
       </c>
+      <c r="S56" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T56" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6987,8 +7329,14 @@
       <c r="R57" t="s">
         <v>703</v>
       </c>
+      <c r="S57" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T57" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -7044,8 +7392,14 @@
       <c r="R58" t="s">
         <v>712</v>
       </c>
+      <c r="S58" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T58" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7101,8 +7455,14 @@
       <c r="R59" t="s">
         <v>721</v>
       </c>
+      <c r="S59" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T59" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7158,8 +7518,14 @@
       <c r="R60" t="s">
         <v>728</v>
       </c>
+      <c r="S60" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T60" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7215,8 +7581,14 @@
       <c r="R61" t="s">
         <v>736</v>
       </c>
+      <c r="S61" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T61" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -7272,8 +7644,14 @@
       <c r="R62" t="s">
         <v>745</v>
       </c>
+      <c r="S62" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T62" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -7329,8 +7707,14 @@
       <c r="R63" t="s">
         <v>752</v>
       </c>
+      <c r="S63" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T63" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -7386,8 +7770,14 @@
       <c r="R64" t="s">
         <v>760</v>
       </c>
+      <c r="S64" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T64" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -7443,8 +7833,14 @@
       <c r="R65" t="s">
         <v>768</v>
       </c>
+      <c r="S65" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T65" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -7500,8 +7896,14 @@
       <c r="R66" t="s">
         <v>776</v>
       </c>
+      <c r="S66" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T66" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -7557,8 +7959,14 @@
       <c r="R67" t="s">
         <v>785</v>
       </c>
+      <c r="S67" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T67" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -7614,8 +8022,14 @@
       <c r="R68" t="s">
         <v>794</v>
       </c>
+      <c r="S68" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T68" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -7671,8 +8085,14 @@
       <c r="R69" t="s">
         <v>803</v>
       </c>
+      <c r="S69" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T69" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -7728,8 +8148,14 @@
       <c r="R70" t="s">
         <v>813</v>
       </c>
+      <c r="S70" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T70" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -7785,8 +8211,14 @@
       <c r="R71" t="s">
         <v>822</v>
       </c>
+      <c r="S71" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T71" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -7842,8 +8274,14 @@
       <c r="R72" t="s">
         <v>827</v>
       </c>
+      <c r="S72" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T72" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -7899,8 +8337,14 @@
       <c r="R73" t="s">
         <v>836</v>
       </c>
+      <c r="S73" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T73" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7956,8 +8400,14 @@
       <c r="R74" t="s">
         <v>845</v>
       </c>
+      <c r="S74" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T74" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -8013,8 +8463,14 @@
       <c r="R75" t="s">
         <v>855</v>
       </c>
+      <c r="S75" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T75" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -8070,8 +8526,14 @@
       <c r="R76" t="s">
         <v>863</v>
       </c>
+      <c r="S76" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T76" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -8127,8 +8589,14 @@
       <c r="R77" t="s">
         <v>871</v>
       </c>
+      <c r="S77" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T77" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -8184,8 +8652,14 @@
       <c r="R78" t="s">
         <v>141</v>
       </c>
+      <c r="S78" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T78" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -8241,8 +8715,14 @@
       <c r="R79" t="s">
         <v>879</v>
       </c>
+      <c r="S79" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T79" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -8298,8 +8778,14 @@
       <c r="R80" t="s">
         <v>888</v>
       </c>
+      <c r="S80" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T80" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -8355,8 +8841,14 @@
       <c r="R81" t="s">
         <v>897</v>
       </c>
+      <c r="S81" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T81" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -8377,7 +8869,7 @@
         <v xml:space="preserve">Statistics &amp; Data Analysis    </v>
       </c>
       <c r="G82" t="s">
-        <v>1104</v>
+        <v>987</v>
       </c>
       <c r="H82" t="s">
         <v>284</v>
@@ -8412,8 +8904,14 @@
       <c r="R82" t="s">
         <v>905</v>
       </c>
+      <c r="S82" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T82" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -8469,8 +8967,14 @@
       <c r="R83" t="s">
         <v>913</v>
       </c>
+      <c r="S83" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T83" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -8526,8 +9030,14 @@
       <c r="R84" t="s">
         <v>922</v>
       </c>
+      <c r="S84" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T84" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -8583,8 +9093,14 @@
       <c r="R85" t="s">
         <v>930</v>
       </c>
+      <c r="S85" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T85" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -8640,8 +9156,14 @@
       <c r="R86" t="s">
         <v>939</v>
       </c>
+      <c r="S86" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T86" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -8697,8 +9219,14 @@
       <c r="R87" t="s">
         <v>947</v>
       </c>
+      <c r="S87" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T87" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -8754,8 +9282,14 @@
       <c r="R88" t="s">
         <v>952</v>
       </c>
+      <c r="S88" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T88" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -8810,6 +9344,12 @@
       </c>
       <c r="R89" t="s">
         <v>961</v>
+      </c>
+      <c r="S89" t="s">
+        <v>1106</v>
+      </c>
+      <c r="T89" t="s">
+        <v>1106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>